<commit_message>
✨ new results excel
</commit_message>
<xml_diff>
--- a/results/optimization_results.xlsx
+++ b/results/optimization_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,39 +488,913 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>OG Kush</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>['Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Energizing', 'Glowing', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>28</v>
+      </c>
+      <c r="I2" t="n">
+        <v>163.8000183105469</v>
+      </c>
+      <c r="J2" t="n">
+        <v>135.8000183105469</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>OG Kush</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>['Banana', 'Gasoline', 'Paracetamol', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>31</v>
+      </c>
+      <c r="I3" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J3" t="n">
+        <v>139.8000030517578</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>OG Kush</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['Cuke', 'Banana', 'Gasoline', 'Paracetamol', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>33</v>
+      </c>
+      <c r="I4" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J4" t="n">
+        <v>137.8000030517578</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>OG Kush</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['Banana', 'Gasoline', 'Paracetamol', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>31</v>
+      </c>
+      <c r="I5" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J5" t="n">
+        <v>139.8000030517578</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Sour Diesel</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>100</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['Banana', 'Cuke', 'Horse S*men', 'Mega Bean', 'Iodine', 'V*agra', 'Motor Oil']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Cyclopean', 'Electrifying', 'Jennerising', 'Long-Faced', 'Slippery', 'Thought-Provoking', 'Tropic-Thunder']</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>38</v>
+      </c>
+      <c r="I6" t="n">
+        <v>167.2999877929688</v>
+      </c>
+      <c r="J6" t="n">
+        <v>129.2999877929688</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sour Diesel</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>100</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Refreshing', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>31</v>
+      </c>
+      <c r="I7" t="n">
+        <v>161</v>
+      </c>
+      <c r="J7" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sour Diesel</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Banana', 'Iodine', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>39</v>
+      </c>
+      <c r="I8" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J8" t="n">
+        <v>131.8000030517578</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sour Diesel</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>100</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['Banana', 'Iodine', 'Paracetamol', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>39</v>
+      </c>
+      <c r="I9" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J9" t="n">
+        <v>131.8000030517578</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Green Crack</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>100</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Cuke', 'Gasoline', 'Cuke', 'Mega Bean', 'Chili', 'Battery']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>['Bright-Eyed', 'Cyclopean', 'Foggy', 'Glowing', 'Long-Faced', 'Spicy', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>34</v>
+      </c>
+      <c r="I10" t="n">
+        <v>165.9000091552734</v>
+      </c>
+      <c r="J10" t="n">
+        <v>131.9000091552734</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Green Crack</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>31</v>
+      </c>
+      <c r="I11" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J11" t="n">
+        <v>139.8000030517578</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Green Crack</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>31</v>
+      </c>
+      <c r="I12" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J12" t="n">
+        <v>139.8000030517578</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Green Crack</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Cuke', 'Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Jennerising', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>33</v>
+      </c>
+      <c r="I13" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="J13" t="n">
+        <v>137.8000030517578</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Grandaddy Purple</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>7</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>100</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['Cuke', 'Energy Drink', 'Paracetamol', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Calorie-Dense', 'Cyclopean', 'Foggy', 'Glowing', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>33</v>
+      </c>
+      <c r="I14" t="n">
+        <v>163.0999908447266</v>
+      </c>
+      <c r="J14" t="n">
+        <v>130.0999908447266</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Grandaddy Purple</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['Paracetamol', 'Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Sedating', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>31</v>
+      </c>
+      <c r="I15" t="n">
+        <v>165.2000122070312</v>
+      </c>
+      <c r="J15" t="n">
+        <v>134.2000122070312</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Grandaddy Purple</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D16" t="n">
+        <v>100</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>['Cuke', 'Paracetamol', 'Cuke', 'Gasoline', 'Mega Bean', 'Banana', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Glowing', 'Sedating', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>33</v>
+      </c>
+      <c r="I16" t="n">
+        <v>165.2000122070312</v>
+      </c>
+      <c r="J16" t="n">
+        <v>132.2000122070312</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Grandaddy Purple</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>100</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['Banana', 'Cuke', 'Paracetamol', 'Banana', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery', 'Banana', 'Cuke']</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Cyclopean', 'Glowing', 'Jennerising', 'Sedating', 'Thought-Provoking', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>35</v>
+      </c>
+      <c r="I17" t="n">
+        <v>165.8999938964844</v>
+      </c>
+      <c r="J17" t="n">
+        <v>130.8999938964844</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Meth</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D18" t="n">
+        <v>100</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['Motor Oil', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Foggy', 'Glowing', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>33</v>
+      </c>
+      <c r="I18" t="n">
+        <v>306.6000061035156</v>
+      </c>
+      <c r="J18" t="n">
+        <v>273.6000061035156</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Meth</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D19" t="n">
+        <v>100</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>['Banana', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Horse S*men', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>['Bright-Eyed', 'Cyclopean', 'Electrifying', 'Foggy', 'Glowing', 'Long-Faced', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>38</v>
+      </c>
+      <c r="I19" t="n">
+        <v>340.1999816894531</v>
+      </c>
+      <c r="J19" t="n">
+        <v>302.1999816894531</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Meth</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>100</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>['Motor Oil', 'Banana', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Horse S*men', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Electrifying', 'Glowing', 'Long-Faced', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>44</v>
+      </c>
+      <c r="I20" t="n">
+        <v>352.7999877929688</v>
+      </c>
+      <c r="J20" t="n">
+        <v>308.7999877929688</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Meth</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>10</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>100</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>['Banana', 'Motor Oil', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Horse S*men', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Electrifying', 'Glowing', 'Long-Faced', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>44</v>
+      </c>
+      <c r="I21" t="n">
+        <v>352.7999877929688</v>
+      </c>
+      <c r="J21" t="n">
+        <v>308.7999877929688</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>Cocaine</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>200</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.999</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>['Banana', 'Cuke', 'Gasoline', 'Mouth Wash', 'Battery', 'Donut', 'Horse S*men', 'Cuke', 'Iodine', 'Mega Bean', 'Energy Drink', 'Cuke', 'Motor Oil']</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Electrifying', 'Long-Faced', 'Shrinking', 'Thought-Provoking', 'Zombifying']</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>64</v>
-      </c>
-      <c r="I2" t="n">
-        <v>771</v>
-      </c>
-      <c r="J2" t="n">
-        <v>707</v>
+      <c r="B22" t="n">
+        <v>7</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['Motor Oil', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Foggy', 'Glowing', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>33</v>
+      </c>
+      <c r="I22" t="n">
+        <v>657</v>
+      </c>
+      <c r="J22" t="n">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Cocaine</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>8</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>100</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>['Horse S*men', 'Motor Oil', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Mega Bean', 'Battery']</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Foggy', 'Glowing', 'Long-Faced', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>42</v>
+      </c>
+      <c r="I23" t="n">
+        <v>734.9999389648438</v>
+      </c>
+      <c r="J23" t="n">
+        <v>692.9999389648438</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Cocaine</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>9</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>100</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>['Banana', 'Motor Oil', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Horse S*men', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Electrifying', 'Glowing', 'Long-Faced', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>44</v>
+      </c>
+      <c r="I24" t="n">
+        <v>756</v>
+      </c>
+      <c r="J24" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Cocaine</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>100</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>['Banana', 'Motor Oil', 'Cuke', 'Paracetamol', 'Gasoline', 'Cuke', 'Battery', 'Horse S*men', 'Mega Bean']</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>['Anti-Gravity', 'Bright-Eyed', 'Cyclopean', 'Electrifying', 'Glowing', 'Long-Faced', 'Tropic-Thunder', 'Zombifying']</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>44</v>
+      </c>
+      <c r="I25" t="n">
+        <v>756</v>
+      </c>
+      <c r="J25" t="n">
+        <v>712</v>
       </c>
     </row>
   </sheetData>

</xml_diff>